<commit_message>
fixes on some formulas
</commit_message>
<xml_diff>
--- a/spot-trade-history.xlsx
+++ b/spot-trade-history.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="48">
   <si>
     <t>BTCUSDT</t>
   </si>
@@ -60,9 +60,6 @@
     <t>BUY</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>19/10/2021</t>
   </si>
   <si>
@@ -87,12 +84,18 @@
     <t>10/05/2022</t>
   </si>
   <si>
+    <t>G13 + H14</t>
+  </si>
+  <si>
     <t>ETHUSDT</t>
   </si>
   <si>
     <t>12/09/2021</t>
   </si>
   <si>
+    <t>G11 + H12</t>
+  </si>
+  <si>
     <t>SOLUSDT</t>
   </si>
   <si>
@@ -117,12 +120,18 @@
     <t>21/10/2021</t>
   </si>
   <si>
+    <t>G17 + H18</t>
+  </si>
+  <si>
     <t>ADAUSDT</t>
   </si>
   <si>
     <t>11/09/2021</t>
   </si>
   <si>
+    <t>G9 + H10</t>
+  </si>
+  <si>
     <t>DOTUSDT</t>
   </si>
   <si>
@@ -135,6 +144,9 @@
     <t>10/11/2021</t>
   </si>
   <si>
+    <t>G15 + H16</t>
+  </si>
+  <si>
     <t>FTMUSDT</t>
   </si>
   <si>
@@ -148,15 +160,21 @@
   </si>
   <si>
     <t>04/01/2022</t>
+  </si>
+  <si>
+    <t>G12 + H13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="$#,##0.00"/>
     <numFmt numFmtId="164" formatCode="$#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
+    <numFmt numFmtId="164" formatCode="$#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -231,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -243,6 +261,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -605,7 +632,7 @@
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -624,7 +651,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2">
-        <v>29119.87</v>
+        <v>30166.73</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -694,24 +721,28 @@
         <v>29.6072532</v>
       </c>
       <c r="F5" s="3">
-        <v>0.00063</v>
+        <f>SUM($D$5:D5)</f>
+        <v>0</v>
       </c>
       <c r="G5" s="4">
-        <v>29.6072532</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E5)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <f>$A$2 * D5 - E5</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <f>H5 / E5</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="C6" s="4">
         <v>61856.47</v>
@@ -723,21 +754,25 @@
         <v>-38.3510114</v>
       </c>
       <c r="F6" s="3">
-        <v>1.000000000000003E-05</v>
+        <f>SUM($D$5:D6)</f>
+        <v>0</v>
       </c>
       <c r="G6" s="4">
-        <v>-8.743758199999995</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E6)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <f>$A$2 * D6 - E6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <f>H6 / E6</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>12</v>
@@ -752,21 +787,25 @@
         <v>99.825</v>
       </c>
       <c r="F7" s="3">
-        <v>0.00166</v>
+        <f>SUM($D$5:D7)</f>
+        <v>0</v>
       </c>
       <c r="G7" s="4">
-        <v>91.08124180000002</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E7)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <f>$A$2 * D7 - E7</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <f>H7 / E7</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>12</v>
@@ -781,21 +820,25 @@
         <v>99.5579</v>
       </c>
       <c r="F8" s="3">
-        <v>0.00335</v>
+        <f>SUM($D$5:D8)</f>
+        <v>0</v>
       </c>
       <c r="G8" s="4">
-        <v>190.6391418</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E8)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <f>$A$2 * D8 - E8</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <f>H8 / E8</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>12</v>
@@ -810,21 +853,25 @@
         <v>149.71205</v>
       </c>
       <c r="F9" s="3">
-        <v>0.007</v>
+        <f>SUM($D$5:D9)</f>
+        <v>0</v>
       </c>
       <c r="G9" s="4">
-        <v>340.3511918</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <f>$A$2 * D9 - E9</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <f>H9 / E9</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>12</v>
@@ -839,21 +886,25 @@
         <v>99.9867204</v>
       </c>
       <c r="F10" s="3">
-        <v>0.009520000000000001</v>
+        <f>SUM($D$5:D10)</f>
+        <v>0</v>
       </c>
       <c r="G10" s="4">
-        <v>440.3379122</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E10)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <f>$A$2 * D10 - E10</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <f>H10 / E10</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>12</v>
@@ -868,24 +919,28 @@
         <v>99.71942400000002</v>
       </c>
       <c r="F11" s="3">
-        <v>0.01208</v>
+        <f>SUM($D$5:D11)</f>
+        <v>0</v>
       </c>
       <c r="G11" s="4">
-        <v>540.0573362</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E11)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <f>$A$2 * D11 - E11</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <f>H11 / E11</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="4">
         <v>30829.51</v>
@@ -897,21 +952,25 @@
         <v>-372.1121857</v>
       </c>
       <c r="F12" s="3">
-        <v>9.999999999999593E-06</v>
+        <f>SUM($D$5:D12)</f>
+        <v>0</v>
       </c>
       <c r="G12" s="4">
-        <v>167.9451505</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E12)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <f>$A$2 * D12 - E12</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <f>H12 / E12</f>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>12</v>
@@ -926,29 +985,44 @@
         <v>374.8834695</v>
       </c>
       <c r="F13" s="3">
-        <v>0.01228</v>
+        <f>SUM($D$5:D13)</f>
+        <v>0</v>
       </c>
       <c r="G13" s="4">
-        <v>542.82862</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E13)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <f>$A$2 * D13 - E13</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <f>H13 / E13</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="C14" s="4">
+      <c r="C14" s="6">
         <f>SUMPRODUCT( C5:C13,D5:D13 ) / SUM(D5:D13)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="1">
         <f>SUM(D5:D13)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="4">
-        <f>SUMPRODUCT( E5:E13,D5:D13 ) / SUM(D5:D13)</f>
+      <c r="E14" s="6">
+        <f>SUM(E5:E13)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="6">
+        <f>SUM(H5:H13)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="7">
+        <f>SUMPRODUCT( I5:I13,D5:D13 ) / SUM(D5:D13)</f>
         <v>0</v>
       </c>
     </row>
@@ -985,7 +1059,7 @@
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1004,7 +1078,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2">
-        <v>29119.89</v>
+        <v>2032.97</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1074,16 +1148,20 @@
         <v>29.735034</v>
       </c>
       <c r="F5" s="3">
-        <v>0.008699999999999999</v>
+        <f>SUM($D$5:D5)</f>
+        <v>0</v>
       </c>
       <c r="G5" s="4">
-        <v>29.735034</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E5)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <f>$A$2 * D5 - E5</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <f>H5 / E5</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1103,24 +1181,28 @@
         <v>24.695592</v>
       </c>
       <c r="F6" s="3">
-        <v>0.0163</v>
+        <f>SUM($D$5:D6)</f>
+        <v>0</v>
       </c>
       <c r="G6" s="4">
-        <v>54.430626</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E6)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <f>$A$2 * D6 - E6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <f>H6 / E6</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="C7" s="4">
         <v>3791</v>
@@ -1132,21 +1214,25 @@
         <v>-61.41419999999999</v>
       </c>
       <c r="F7" s="3">
-        <v>9.999999999999939E-05</v>
+        <f>SUM($D$5:D7)</f>
+        <v>0</v>
       </c>
       <c r="G7" s="4">
-        <v>-6.98357399999999</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E7)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <f>$A$2 * D7 - E7</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <f>H7 / E7</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>12</v>
@@ -1161,24 +1247,28 @@
         <v>99.696</v>
       </c>
       <c r="F8" s="3">
-        <v>0.0249</v>
+        <f>SUM($D$5:D8)</f>
+        <v>0</v>
       </c>
       <c r="G8" s="4">
-        <v>92.71242600000001</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E8)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <f>$A$2 * D8 - E8</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <f>H8 / E8</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="4">
         <v>2223.18</v>
@@ -1190,24 +1280,28 @@
         <v>-99.82078199999999</v>
       </c>
       <c r="F9" s="3">
-        <v>-0.02</v>
+        <f>SUM($D$5:D9)</f>
+        <v>0</v>
       </c>
       <c r="G9" s="4">
-        <v>-7.108355999999986</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <f>$A$2 * D9 - E9</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <f>H9 / E9</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="4">
         <v>2326.09</v>
@@ -1219,21 +1313,25 @@
         <v>-99.78926100000001</v>
       </c>
       <c r="F10" s="3">
-        <v>-0.06290000000000001</v>
+        <f>SUM($D$5:D10)</f>
+        <v>0</v>
       </c>
       <c r="G10" s="4">
-        <v>-106.897617</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E10)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <f>$A$2 * D10 - E10</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <f>H10 / E10</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>12</v>
@@ -1248,29 +1346,44 @@
         <v>199.909212</v>
       </c>
       <c r="F11" s="3">
-        <v>0.02499999999999999</v>
+        <f>SUM($D$5:D11)</f>
+        <v>0</v>
       </c>
       <c r="G11" s="4">
-        <v>93.01159500000003</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E11)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <f>$A$2 * D11 - E11</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <f>H11 / E11</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="C12" s="4">
+      <c r="C12" s="6">
         <f>SUMPRODUCT( C5:C11,D5:D11 ) / SUM(D5:D11)</f>
         <v>0</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="1">
         <f>SUM(D5:D11)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="4">
-        <f>SUMPRODUCT( E5:E11,D5:D11 ) / SUM(D5:D11)</f>
+      <c r="E12" s="6">
+        <f>SUM(E5:E11)</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="6">
+        <f>SUM(H5:H11)</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="7">
+        <f>SUMPRODUCT( I5:I11,D5:D11 ) / SUM(D5:D11)</f>
         <v>0</v>
       </c>
     </row>
@@ -1307,13 +1420,13 @@
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1326,7 +1439,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2">
-        <v>29119.89</v>
+        <v>51.68</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1381,7 +1494,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>12</v>
@@ -1396,24 +1509,28 @@
         <v>18.7299</v>
       </c>
       <c r="F5" s="3">
-        <v>0.09</v>
+        <f>SUM($D$5:D5)</f>
+        <v>0</v>
       </c>
       <c r="G5" s="4">
-        <v>18.7299</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E5)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <f>$A$2 * D5 - E5</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <f>H5 / E5</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4">
         <v>211.47</v>
@@ -1425,21 +1542,25 @@
         <v>-16.9176</v>
       </c>
       <c r="F6" s="3">
-        <v>0.009999999999999995</v>
+        <f>SUM($D$5:D6)</f>
+        <v>0</v>
       </c>
       <c r="G6" s="4">
-        <v>1.8123</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E6)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <f>$A$2 * D6 - E6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <f>H6 / E6</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>12</v>
@@ -1454,24 +1575,28 @@
         <v>48.8722</v>
       </c>
       <c r="F7" s="3">
-        <v>0.27</v>
+        <f>SUM($D$5:D7)</f>
+        <v>0</v>
       </c>
       <c r="G7" s="4">
-        <v>50.6845</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E7)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <f>$A$2 * D7 - E7</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <f>H7 / E7</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4">
         <v>194.25</v>
@@ -1483,21 +1608,25 @@
         <v>-50.505</v>
       </c>
       <c r="F8" s="3">
-        <v>0.01000000000000001</v>
+        <f>SUM($D$5:D8)</f>
+        <v>0</v>
       </c>
       <c r="G8" s="4">
-        <v>0.1794999999999973</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E8)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <f>$A$2 * D8 - E8</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <f>H8 / E8</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>12</v>
@@ -1512,21 +1641,25 @@
         <v>44.6407</v>
       </c>
       <c r="F9" s="3">
-        <v>0.24</v>
+        <f>SUM($D$5:D9)</f>
+        <v>0</v>
       </c>
       <c r="G9" s="4">
-        <v>44.8202</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <f>$A$2 * D9 - E9</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <f>H9 / E9</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>12</v>
@@ -1541,21 +1674,25 @@
         <v>28.6704</v>
       </c>
       <c r="F10" s="3">
-        <v>0.42</v>
+        <f>SUM($D$5:D10)</f>
+        <v>0</v>
       </c>
       <c r="G10" s="4">
-        <v>73.4906</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E10)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <f>$A$2 * D10 - E10</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <f>H10 / E10</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>12</v>
@@ -1570,21 +1707,25 @@
         <v>31.464</v>
       </c>
       <c r="F11" s="3">
-        <v>0.6200000000000001</v>
+        <f>SUM($D$5:D11)</f>
+        <v>0</v>
       </c>
       <c r="G11" s="4">
-        <v>104.9546</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E11)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <f>$A$2 * D11 - E11</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <f>H11 / E11</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>12</v>
@@ -1599,21 +1740,25 @@
         <v>228.114</v>
       </c>
       <c r="F12" s="3">
-        <v>2.07</v>
+        <f>SUM($D$5:D12)</f>
+        <v>0</v>
       </c>
       <c r="G12" s="4">
-        <v>333.0685999999999</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E12)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <f>$A$2 * D12 - E12</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <f>H12 / E12</f>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>12</v>
@@ -1628,21 +1773,25 @@
         <v>49.9932</v>
       </c>
       <c r="F13" s="3">
-        <v>2.43</v>
+        <f>SUM($D$5:D13)</f>
+        <v>0</v>
       </c>
       <c r="G13" s="4">
-        <v>383.0617999999999</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E13)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <f>$A$2 * D13 - E13</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <f>H13 / E13</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>12</v>
@@ -1657,24 +1806,28 @@
         <v>226.9533</v>
       </c>
       <c r="F14" s="3">
-        <v>3.9</v>
+        <f>SUM($D$5:D14)</f>
+        <v>0</v>
       </c>
       <c r="G14" s="4">
-        <v>610.0151</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E14)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <f>$A$2 * D14 - E14</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <f>H14 / E14</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="C15" s="4">
         <v>157.19</v>
@@ -1686,24 +1839,28 @@
         <v>-99.02970000000001</v>
       </c>
       <c r="F15" s="3">
-        <v>3.27</v>
+        <f>SUM($D$5:D15)</f>
+        <v>0</v>
       </c>
       <c r="G15" s="4">
-        <v>510.9854</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E15)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <f>$A$2 * D15 - E15</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <f>H15 / E15</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="4">
         <v>184</v>
@@ -1715,24 +1872,28 @@
         <v>-108.56</v>
       </c>
       <c r="F16" s="3">
-        <v>2.680000000000001</v>
+        <f>SUM($D$5:D16)</f>
+        <v>0</v>
       </c>
       <c r="G16" s="4">
-        <v>402.4254</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E16)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <f>$A$2 * D16 - E16</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <f>H16 / E16</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="4">
         <v>181</v>
@@ -1744,29 +1905,44 @@
         <v>-108.6</v>
       </c>
       <c r="F17" s="3">
-        <v>2.080000000000001</v>
+        <f>SUM($D$5:D17)</f>
+        <v>0</v>
       </c>
       <c r="G17" s="4">
-        <v>293.8253999999999</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E17)</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <f>$A$2 * D17 - E17</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <f>H17 / E17</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="C18" s="4">
+      <c r="C18" s="6">
         <f>SUMPRODUCT( C5:C17,D5:D17 ) / SUM(D5:D17)</f>
         <v>0</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="1">
         <f>SUM(D5:D17)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="4">
-        <f>SUMPRODUCT( E5:E17,D5:D17 ) / SUM(D5:D17)</f>
+      <c r="E18" s="6">
+        <f>SUM(E5:E17)</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="6">
+        <f>SUM(H5:H17)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="7">
+        <f>SUMPRODUCT( I5:I17,D5:D17 ) / SUM(D5:D17)</f>
         <v>0</v>
       </c>
     </row>
@@ -1803,13 +1979,13 @@
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1822,7 +1998,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2">
-        <v>29120.03</v>
+        <v>0.53</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1877,7 +2053,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>12</v>
@@ -1892,21 +2068,25 @@
         <v>29.953</v>
       </c>
       <c r="F5" s="3">
-        <v>11</v>
+        <f>SUM($D$5:D5)</f>
+        <v>0</v>
       </c>
       <c r="G5" s="4">
-        <v>29.953</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E5)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <f>$A$2 * D5 - E5</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <f>H5 / E5</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>12</v>
@@ -1921,21 +2101,25 @@
         <v>49.88480000000001</v>
       </c>
       <c r="F6" s="3">
-        <v>34.8</v>
+        <f>SUM($D$5:D6)</f>
+        <v>0</v>
       </c>
       <c r="G6" s="4">
-        <v>79.8378</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E6)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <f>$A$2 * D6 - E6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <f>H6 / E6</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>12</v>
@@ -1950,21 +2134,25 @@
         <v>74.89919999999999</v>
       </c>
       <c r="F7" s="3">
-        <v>68</v>
+        <f>SUM($D$5:D7)</f>
+        <v>0</v>
       </c>
       <c r="G7" s="4">
-        <v>154.737</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E7)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <f>$A$2 * D7 - E7</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <f>H7 / E7</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>12</v>
@@ -1979,21 +2167,25 @@
         <v>14.2272</v>
       </c>
       <c r="F8" s="3">
-        <v>75.2</v>
+        <f>SUM($D$5:D8)</f>
+        <v>0</v>
       </c>
       <c r="G8" s="4">
-        <v>168.9642</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E8)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <f>$A$2 * D8 - E8</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <f>H8 / E8</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>12</v>
@@ -2008,29 +2200,44 @@
         <v>60.6632</v>
       </c>
       <c r="F9" s="3">
-        <v>105.9</v>
+        <f>SUM($D$5:D9)</f>
+        <v>0</v>
       </c>
       <c r="G9" s="4">
-        <v>229.6274</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <f>$A$2 * D9 - E9</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <f>H9 / E9</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="C10" s="4">
+      <c r="C10" s="6">
         <f>SUMPRODUCT( C5:C9,D5:D9 ) / SUM(D5:D9)</f>
         <v>0</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="1">
         <f>SUM(D5:D9)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="4">
-        <f>SUMPRODUCT( E5:E9,D5:D9 ) / SUM(D5:D9)</f>
+      <c r="E10" s="6">
+        <f>SUM(E5:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="6">
+        <f>SUM(H5:H9)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="7">
+        <f>SUMPRODUCT( I5:I9,D5:D9 ) / SUM(D5:D9)</f>
         <v>0</v>
       </c>
     </row>
@@ -2067,13 +2274,13 @@
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2086,7 +2293,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2">
-        <v>29120.04</v>
+        <v>9.960000000000001</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2156,24 +2363,28 @@
         <v>29.8102</v>
       </c>
       <c r="F5" s="3">
-        <v>1.07</v>
+        <f>SUM($D$5:D5)</f>
+        <v>0</v>
       </c>
       <c r="G5" s="4">
-        <v>29.8102</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E5)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <f>$A$2 * D5 - E5</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <f>H5 / E5</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4">
         <v>29.02</v>
@@ -2185,21 +2396,25 @@
         <v>-30.7612</v>
       </c>
       <c r="F6" s="3">
-        <v>0.01000000000000001</v>
+        <f>SUM($D$5:D6)</f>
+        <v>0</v>
       </c>
       <c r="G6" s="4">
-        <v>-0.9510000000000005</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E6)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <f>$A$2 * D6 - E6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <f>H6 / E6</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>12</v>
@@ -2214,21 +2429,25 @@
         <v>49.6838</v>
       </c>
       <c r="F7" s="3">
-        <v>1.47</v>
+        <f>SUM($D$5:D7)</f>
+        <v>0</v>
       </c>
       <c r="G7" s="4">
-        <v>48.7328</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E7)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <f>$A$2 * D7 - E7</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <f>H7 / E7</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>12</v>
@@ -2243,21 +2462,25 @@
         <v>20.594</v>
       </c>
       <c r="F8" s="3">
-        <v>2.17</v>
+        <f>SUM($D$5:D8)</f>
+        <v>0</v>
       </c>
       <c r="G8" s="4">
-        <v>69.32679999999999</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E8)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <f>$A$2 * D8 - E8</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <f>H8 / E8</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>12</v>
@@ -2272,21 +2495,25 @@
         <v>49.88</v>
       </c>
       <c r="F9" s="3">
-        <v>3.89</v>
+        <f>SUM($D$5:D9)</f>
+        <v>0</v>
       </c>
       <c r="G9" s="4">
-        <v>119.2068</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <f>$A$2 * D9 - E9</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <f>H9 / E9</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>12</v>
@@ -2301,24 +2528,28 @@
         <v>29.9922</v>
       </c>
       <c r="F10" s="3">
-        <v>5</v>
+        <f>SUM($D$5:D10)</f>
+        <v>0</v>
       </c>
       <c r="G10" s="4">
-        <v>149.199</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E10)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <f>$A$2 * D10 - E10</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <f>H10 / E10</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="4">
         <v>35.57</v>
@@ -2330,24 +2561,28 @@
         <v>-3.2013</v>
       </c>
       <c r="F11" s="3">
-        <v>4.91</v>
+        <f>SUM($D$5:D11)</f>
+        <v>0</v>
       </c>
       <c r="G11" s="4">
-        <v>145.9977</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E11)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <f>$A$2 * D11 - E11</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <f>H11 / E11</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="4">
         <v>35.57</v>
@@ -2359,21 +2594,25 @@
         <v>-174.293</v>
       </c>
       <c r="F12" s="3">
-        <v>0.009999999999999787</v>
+        <f>SUM($D$5:D12)</f>
+        <v>0</v>
       </c>
       <c r="G12" s="4">
-        <v>-28.29530000000003</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E12)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <f>$A$2 * D12 - E12</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <f>H12 / E12</f>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>12</v>
@@ -2388,21 +2627,25 @@
         <v>50.5</v>
       </c>
       <c r="F13" s="3">
-        <v>1.01</v>
+        <f>SUM($D$5:D13)</f>
+        <v>0</v>
       </c>
       <c r="G13" s="4">
-        <v>22.20469999999997</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E13)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <f>$A$2 * D13 - E13</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <f>H13 / E13</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>12</v>
@@ -2417,21 +2660,25 @@
         <v>99.50080000000001</v>
       </c>
       <c r="F14" s="3">
-        <v>3.25</v>
+        <f>SUM($D$5:D14)</f>
+        <v>0</v>
       </c>
       <c r="G14" s="4">
-        <v>121.7055</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E14)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <f>$A$2 * D14 - E14</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <f>H14 / E14</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>12</v>
@@ -2446,29 +2693,44 @@
         <v>99.9798</v>
       </c>
       <c r="F15" s="3">
-        <v>8.870000000000001</v>
+        <f>SUM($D$5:D15)</f>
+        <v>0</v>
       </c>
       <c r="G15" s="4">
-        <v>221.6853</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E15)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <f>$A$2 * D15 - E15</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <f>H15 / E15</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="C16" s="4">
+      <c r="C16" s="6">
         <f>SUMPRODUCT( C5:C15,D5:D15 ) / SUM(D5:D15)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="1">
         <f>SUM(D5:D15)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="4">
-        <f>SUMPRODUCT( E5:E15,D5:D15 ) / SUM(D5:D15)</f>
+      <c r="E16" s="6">
+        <f>SUM(E5:E15)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="6">
+        <f>SUM(H5:H15)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="7">
+        <f>SUMPRODUCT( I5:I15,D5:D15 ) / SUM(D5:D15)</f>
         <v>0</v>
       </c>
     </row>
@@ -2505,13 +2767,13 @@
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2524,7 +2786,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2">
-        <v>29120.33</v>
+        <v>0.34</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2579,7 +2841,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>12</v>
@@ -2594,24 +2856,28 @@
         <v>29.3964</v>
       </c>
       <c r="F5" s="3">
-        <v>22</v>
+        <f>SUM($D$5:D5)</f>
+        <v>0</v>
       </c>
       <c r="G5" s="4">
-        <v>29.3964</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E5)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <f>$A$2 * D5 - E5</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <f>H5 / E5</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4">
         <v>1.5208</v>
@@ -2623,21 +2889,25 @@
         <v>-31.9368</v>
       </c>
       <c r="F6" s="3">
-        <v>1</v>
+        <f>SUM($D$5:D6)</f>
+        <v>0</v>
       </c>
       <c r="G6" s="4">
-        <v>-2.540399999999998</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E6)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <f>$A$2 * D6 - E6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <f>H6 / E6</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>12</v>
@@ -2652,24 +2922,28 @@
         <v>43.42</v>
       </c>
       <c r="F7" s="3">
-        <v>27</v>
+        <f>SUM($D$5:D7)</f>
+        <v>0</v>
       </c>
       <c r="G7" s="4">
-        <v>40.8796</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E7)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <f>$A$2 * D7 - E7</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <f>H7 / E7</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4">
         <v>1.75</v>
@@ -2681,16 +2955,20 @@
         <v>-45.5</v>
       </c>
       <c r="F8" s="3">
-        <v>1</v>
+        <f>SUM($D$5:D8)</f>
+        <v>0</v>
       </c>
       <c r="G8" s="4">
-        <v>-4.620399999999997</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E8)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <f>$A$2 * D8 - E8</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <f>H8 / E8</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2710,24 +2988,28 @@
         <v>31.8296</v>
       </c>
       <c r="F9" s="3">
-        <v>23</v>
+        <f>SUM($D$5:D9)</f>
+        <v>0</v>
       </c>
       <c r="G9" s="4">
-        <v>27.20920000000001</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <f>$A$2 * D9 - E9</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <f>H9 / E9</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="4">
         <v>2.2999</v>
@@ -2739,21 +3021,25 @@
         <v>-50.5978</v>
       </c>
       <c r="F10" s="3">
-        <v>1</v>
+        <f>SUM($D$5:D10)</f>
+        <v>0</v>
       </c>
       <c r="G10" s="4">
-        <v>-23.38859999999999</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E10)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <f>$A$2 * D10 - E10</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <f>H10 / E10</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>12</v>
@@ -2768,24 +3054,28 @@
         <v>52.624</v>
       </c>
       <c r="F11" s="3">
-        <v>21</v>
+        <f>SUM($D$5:D11)</f>
+        <v>0</v>
       </c>
       <c r="G11" s="4">
-        <v>29.23540000000001</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E11)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <f>$A$2 * D11 - E11</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <f>H11 / E11</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="4">
         <v>2.8383</v>
@@ -2797,29 +3087,44 @@
         <v>-56.766</v>
       </c>
       <c r="F12" s="3">
-        <v>1</v>
+        <f>SUM($D$5:D12)</f>
+        <v>0</v>
       </c>
       <c r="G12" s="4">
-        <v>-27.53059999999999</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>13</v>
+        <f>SUM($E$5:E12)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <f>$A$2 * D12 - E12</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <f>H12 / E12</f>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="C13" s="4">
+      <c r="C13" s="6">
         <f>SUMPRODUCT( C5:C12,D5:D12 ) / SUM(D5:D12)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="1">
         <f>SUM(D5:D12)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="4">
-        <f>SUMPRODUCT( E5:E12,D5:D12 ) / SUM(D5:D12)</f>
+      <c r="E13" s="6">
+        <f>SUM(E5:E12)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="6">
+        <f>SUM(H5:H12)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="7">
+        <f>SUMPRODUCT( I5:I12,D5:D12 ) / SUM(D5:D12)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>